<commit_message>
Create data sources table
</commit_message>
<xml_diff>
--- a/Sources/Data_sources.xlsx
+++ b/Sources/Data_sources.xlsx
@@ -23,12 +23,67 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Bathymetry</t>
+  </si>
+  <si>
+    <t>poster</t>
+  </si>
+  <si>
+    <t>Irradiance</t>
+  </si>
+  <si>
+    <t>Lake Washington WQ</t>
+  </si>
+  <si>
+    <t>Lake Washington meteorology</t>
+  </si>
+  <si>
+    <t>King County buoy</t>
+  </si>
+  <si>
+    <t>Citation</t>
+  </si>
+  <si>
+    <t>https://green2.kingcounty.gov/lake-buoy/Data.aspx</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Smoke data</t>
+  </si>
+  <si>
+    <t>NOAA</t>
+  </si>
+  <si>
+    <t>https://satepsanone.nesdis.noaa.gov/pub/volcano/FIRE/HMS_ARCHIVE/</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -51,13 +106,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,12 +394,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added satellite data description
</commit_message>
<xml_diff>
--- a/Sources/Data_sources.xlsx
+++ b/Sources/Data_sources.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jane Fencl\Documents\Jane_Stuff_UW\UW_Research\Data\Lake_WA\Lake_WA\Sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanr\OneDrive\uw\Research Derby\repo\Research-Derby\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_59BEDC77F10A9CE6573157F12329EAF7366C62E1" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D73AED42-B1F4-4369-80BA-25D4B93D92EF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17820" windowHeight="11310"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="21600" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Data</t>
   </si>
@@ -66,12 +67,30 @@
   </si>
   <si>
     <t>https://satepsanone.nesdis.noaa.gov/pub/volcano/FIRE/HMS_ARCHIVE/</t>
+  </si>
+  <si>
+    <t>https://disc.gsfc.nasa.gov/datasets/OMPS_NPP_NMTO3_L3_DAILY_2/summary</t>
+  </si>
+  <si>
+    <t>UV Aerosol Index - OMPS-NPP NMTO3 L2 v2.1</t>
+  </si>
+  <si>
+    <t>NASA GES DIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hourly Cloud Optical Depth - SATCORPS CERES GEO GOES-15 Ed 4 v1.0, v1.2 </t>
+  </si>
+  <si>
+    <t>NOAA/NASA LARC DAP</t>
+  </si>
+  <si>
+    <t>https://opendap.larc.nasa.gov/opendap/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,11 +412,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,11 +485,35 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{93A16DA7-7D26-4199-B61A-F3AE13D588C3}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{FCED780F-DB75-405D-8230-340775ACEA2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>